<commit_message>
request.py for web search and catch item
</commit_message>
<xml_diff>
--- a/myfile/myels.xlsx
+++ b/myfile/myels.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B4:B4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,10 +421,111 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>類別</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>編號</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>品名</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>單價</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>單位</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>蔬菜</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>高麗菜</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>粒</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>水果</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>草莓</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>箱</t>
+        </is>
+      </c>
+    </row>
     <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>堅果</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>try</t>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>杏仁</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>罐</t>
         </is>
       </c>
     </row>

</xml_diff>